<commit_message>
Added some trims to prohibit often happening error of whitespaces
</commit_message>
<xml_diff>
--- a/src/test/resources/visitExcelActivitySplitSubgroupValuesTest.xlsx
+++ b/src/test/resources/visitExcelActivitySplitSubgroupValuesTest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Manu/IdeaProjects/MetaDBRestAPIPadim/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DED17A87-A9A6-BC49-8D0F-5004358E3755}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1C7CC66-7161-AC41-80E0-B0DC7D7E649A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1323,7 +1323,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C22" sqref="C22"/>
+      <selection pane="bottomRight" activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>